<commit_message>
Update on 20250117 part 5
</commit_message>
<xml_diff>
--- a/各地组播源汇总/上海.xlsx
+++ b/各地组播源汇总/上海.xlsx
@@ -12,7 +12,7 @@
     <sheet name="可用IP地址" sheetId="12" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">电信组播!$A$1:$E$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">电信组播!$A$1:$F$167</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">移动itv!$A$1:$E$1105</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6058" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6555" uniqueCount="281">
   <si>
     <t>电信组播</t>
   </si>
@@ -665,9 +665,6 @@
     <t>风云音乐</t>
   </si>
   <si>
-    <t>文化精品</t>
-  </si>
-  <si>
     <t>CCTV-4K</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -726,9 +723,6 @@
     <t>/udp/239.45.0.54:5140</t>
   </si>
   <si>
-    <t>央视高网</t>
-  </si>
-  <si>
     <t>CETV-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -777,6 +771,138 @@
   </si>
   <si>
     <t>116.227.10.196:2048</t>
+  </si>
+  <si>
+    <t>/udp/239.45.3.61:5140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/udp/233.18.204.51:5140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/udp/239.45.3.209:5140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/udp/233.18.204.57:5140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/udp/239.45.3.236:5140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/udp/233.18.204.53:5140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>央视文化精品</t>
+  </si>
+  <si>
+    <t>高尔夫网球</t>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$上海电信</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/udp/239.45.1.17:5140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/udp/233.18.204.55:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.59:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.58:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.54:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.63:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.47:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.66:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.49:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.65:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.115:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.48:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.46:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.45:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.44:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.175:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.173:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.174:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.188:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.187:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.176:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.180:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.184:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.183:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.185:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.182:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.181:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.186:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.179:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.177:5140</t>
+  </si>
+  <si>
+    <t>/udp/233.18.204.178:5140</t>
   </si>
 </sst>
 </file>
@@ -19949,7 +20075,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E541"/>
+  <dimension ref="A1:F605"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19959,10 +20085,11 @@
     <col min="2" max="2" width="7.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -19978,8 +20105,11 @@
       <c r="E1" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F1" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>134</v>
       </c>
@@ -19995,8 +20125,11 @@
       <c r="E2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>134</v>
       </c>
@@ -20012,8 +20145,11 @@
       <c r="E3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>134</v>
       </c>
@@ -20029,8 +20165,11 @@
       <c r="E4" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>134</v>
       </c>
@@ -20044,12 +20183,15 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+        <v>240</v>
+      </c>
+      <c r="F5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>25</v>
@@ -20061,12 +20203,15 @@
         <v>135</v>
       </c>
       <c r="E6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+        <v>241</v>
+      </c>
+      <c r="F6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
@@ -20078,12 +20223,15 @@
         <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+        <v>241</v>
+      </c>
+      <c r="F7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>140</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>25</v>
@@ -20095,12 +20243,15 @@
         <v>135</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+        <v>138</v>
+      </c>
+      <c r="F8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>140</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>25</v>
@@ -20112,12 +20263,15 @@
         <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+        <v>242</v>
+      </c>
+      <c r="F9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>141</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>25</v>
@@ -20129,12 +20283,15 @@
         <v>135</v>
       </c>
       <c r="E10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+        <v>243</v>
+      </c>
+      <c r="F10" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>141</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>25</v>
@@ -20146,12 +20303,15 @@
         <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+        <v>243</v>
+      </c>
+      <c r="F11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>25</v>
@@ -20163,12 +20323,15 @@
         <v>135</v>
       </c>
       <c r="E12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+        <v>139</v>
+      </c>
+      <c r="F12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>25</v>
@@ -20180,12 +20343,15 @@
         <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+        <v>244</v>
+      </c>
+      <c r="F13" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>1</v>
+        <v>140</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>25</v>
@@ -20197,12 +20363,15 @@
         <v>135</v>
       </c>
       <c r="E14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+        <v>245</v>
+      </c>
+      <c r="F14" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>1</v>
+        <v>140</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>25</v>
@@ -20214,12 +20383,15 @@
         <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+        <v>245</v>
+      </c>
+      <c r="F15" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>141</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>25</v>
@@ -20231,12 +20403,15 @@
         <v>135</v>
       </c>
       <c r="E16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+        <v>142</v>
+      </c>
+      <c r="F16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>141</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>25</v>
@@ -20248,12 +20423,15 @@
         <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+        <v>142</v>
+      </c>
+      <c r="F17" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>25</v>
@@ -20265,12 +20443,15 @@
         <v>135</v>
       </c>
       <c r="E18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+        <v>143</v>
+      </c>
+      <c r="F18" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>25</v>
@@ -20282,12 +20463,15 @@
         <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+        <v>143</v>
+      </c>
+      <c r="F19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>25</v>
@@ -20299,12 +20483,15 @@
         <v>135</v>
       </c>
       <c r="E20" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+        <v>251</v>
+      </c>
+      <c r="F20" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>25</v>
@@ -20316,12 +20503,15 @@
         <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+        <v>251</v>
+      </c>
+      <c r="F21" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>25</v>
@@ -20333,12 +20523,15 @@
         <v>135</v>
       </c>
       <c r="E22" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+        <v>144</v>
+      </c>
+      <c r="F22" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>25</v>
@@ -20350,12 +20543,15 @@
         <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+        <v>144</v>
+      </c>
+      <c r="F23" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>25</v>
@@ -20367,12 +20563,15 @@
         <v>135</v>
       </c>
       <c r="E24" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+        <v>252</v>
+      </c>
+      <c r="F24" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>25</v>
@@ -20384,12 +20583,15 @@
         <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+        <v>252</v>
+      </c>
+      <c r="F25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>25</v>
@@ -20401,12 +20603,15 @@
         <v>135</v>
       </c>
       <c r="E26" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+      <c r="F26" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>25</v>
@@ -20418,12 +20623,15 @@
         <v>31</v>
       </c>
       <c r="E27" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+      <c r="F27" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>25</v>
@@ -20435,12 +20643,15 @@
         <v>135</v>
       </c>
       <c r="E28" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+        <v>253</v>
+      </c>
+      <c r="F28" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>25</v>
@@ -20452,12 +20663,15 @@
         <v>31</v>
       </c>
       <c r="E29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+        <v>253</v>
+      </c>
+      <c r="F29" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>25</v>
@@ -20469,12 +20683,15 @@
         <v>135</v>
       </c>
       <c r="E30" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+        <v>146</v>
+      </c>
+      <c r="F30" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>25</v>
@@ -20486,12 +20703,15 @@
         <v>31</v>
       </c>
       <c r="E31" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+        <v>146</v>
+      </c>
+      <c r="F31" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>25</v>
@@ -20503,12 +20723,15 @@
         <v>135</v>
       </c>
       <c r="E32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+        <v>254</v>
+      </c>
+      <c r="F32" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>25</v>
@@ -20520,12 +20743,15 @@
         <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+        <v>254</v>
+      </c>
+      <c r="F33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>25</v>
@@ -20537,12 +20763,15 @@
         <v>135</v>
       </c>
       <c r="E34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+        <v>147</v>
+      </c>
+      <c r="F34" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>25</v>
@@ -20554,12 +20783,15 @@
         <v>31</v>
       </c>
       <c r="E35" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+        <v>147</v>
+      </c>
+      <c r="F35" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>25</v>
@@ -20571,12 +20803,15 @@
         <v>135</v>
       </c>
       <c r="E36" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+        <v>148</v>
+      </c>
+      <c r="F36" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>25</v>
@@ -20588,12 +20823,15 @@
         <v>31</v>
       </c>
       <c r="E37" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+        <v>148</v>
+      </c>
+      <c r="F37" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>25</v>
@@ -20605,12 +20843,15 @@
         <v>135</v>
       </c>
       <c r="E38" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+        <v>255</v>
+      </c>
+      <c r="F38" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>25</v>
@@ -20622,12 +20863,15 @@
         <v>31</v>
       </c>
       <c r="E39" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+        <v>255</v>
+      </c>
+      <c r="F39" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>150</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>25</v>
@@ -20639,12 +20883,15 @@
         <v>135</v>
       </c>
       <c r="E40" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+        <v>149</v>
+      </c>
+      <c r="F40" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>8</v>
+        <v>150</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>25</v>
@@ -20656,12 +20903,15 @@
         <v>31</v>
       </c>
       <c r="E41" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+        <v>149</v>
+      </c>
+      <c r="F41" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>7</v>
+        <v>150</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>25</v>
@@ -20673,12 +20923,15 @@
         <v>135</v>
       </c>
       <c r="E42" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+        <v>256</v>
+      </c>
+      <c r="F42" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>7</v>
+        <v>150</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>25</v>
@@ -20690,12 +20943,15 @@
         <v>31</v>
       </c>
       <c r="E43" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+        <v>256</v>
+      </c>
+      <c r="F43" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>25</v>
@@ -20707,12 +20963,15 @@
         <v>135</v>
       </c>
       <c r="E44" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+        <v>151</v>
+      </c>
+      <c r="F44" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>25</v>
@@ -20724,12 +20983,15 @@
         <v>31</v>
       </c>
       <c r="E45" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+        <v>152</v>
+      </c>
+      <c r="F45" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>25</v>
@@ -20741,12 +21003,15 @@
         <v>135</v>
       </c>
       <c r="E46" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+        <v>151</v>
+      </c>
+      <c r="F46" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>25</v>
@@ -20758,12 +21023,15 @@
         <v>31</v>
       </c>
       <c r="E47" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+        <v>152</v>
+      </c>
+      <c r="F47" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>164</v>
+        <v>13</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>25</v>
@@ -20775,12 +21043,15 @@
         <v>135</v>
       </c>
       <c r="E48" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+        <v>257</v>
+      </c>
+      <c r="F48" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>164</v>
+        <v>13</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>25</v>
@@ -20792,12 +21063,15 @@
         <v>31</v>
       </c>
       <c r="E49" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+        <v>257</v>
+      </c>
+      <c r="F49" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>166</v>
+        <v>17</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>25</v>
@@ -20809,12 +21083,15 @@
         <v>135</v>
       </c>
       <c r="E50" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+        <v>153</v>
+      </c>
+      <c r="F50" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>166</v>
+        <v>17</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>25</v>
@@ -20826,12 +21103,15 @@
         <v>31</v>
       </c>
       <c r="E51" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+        <v>153</v>
+      </c>
+      <c r="F51" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>168</v>
+        <v>9</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>25</v>
@@ -20843,12 +21123,15 @@
         <v>135</v>
       </c>
       <c r="E52" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+        <v>154</v>
+      </c>
+      <c r="F52" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>168</v>
+        <v>9</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>25</v>
@@ -20860,12 +21143,15 @@
         <v>31</v>
       </c>
       <c r="E53" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+        <v>154</v>
+      </c>
+      <c r="F53" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>170</v>
+        <v>9</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>25</v>
@@ -20877,12 +21163,15 @@
         <v>135</v>
       </c>
       <c r="E54" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+        <v>258</v>
+      </c>
+      <c r="F54" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>170</v>
+        <v>9</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>25</v>
@@ -20894,12 +21183,15 @@
         <v>31</v>
       </c>
       <c r="E55" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+        <v>258</v>
+      </c>
+      <c r="F55" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>208</v>
+        <v>2</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>25</v>
@@ -20911,12 +21203,15 @@
         <v>135</v>
       </c>
       <c r="E56" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+        <v>155</v>
+      </c>
+      <c r="F56" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>208</v>
+        <v>2</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>25</v>
@@ -20928,12 +21223,15 @@
         <v>31</v>
       </c>
       <c r="E57" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+        <v>155</v>
+      </c>
+      <c r="F57" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>228</v>
+        <v>2</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>25</v>
@@ -20945,12 +21243,15 @@
         <v>135</v>
       </c>
       <c r="E58" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+        <v>259</v>
+      </c>
+      <c r="F58" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>228</v>
+        <v>2</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>25</v>
@@ -20959,32 +21260,38 @@
         <v>26</v>
       </c>
       <c r="D59" t="s">
+        <v>31</v>
+      </c>
+      <c r="E59" t="s">
+        <v>259</v>
+      </c>
+      <c r="F59" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A60" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" t="s">
         <v>135</v>
       </c>
-      <c r="E59" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" t="s">
-        <v>26</v>
-      </c>
-      <c r="D60" t="s">
-        <v>31</v>
-      </c>
       <c r="E60" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+        <v>156</v>
+      </c>
+      <c r="F60" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>228</v>
+        <v>158</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>25</v>
@@ -20996,12 +21303,15 @@
         <v>31</v>
       </c>
       <c r="E61" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+        <v>157</v>
+      </c>
+      <c r="F61" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>229</v>
+        <v>158</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>25</v>
@@ -21013,12 +21323,15 @@
         <v>135</v>
       </c>
       <c r="E62" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+        <v>156</v>
+      </c>
+      <c r="F62" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>229</v>
+        <v>158</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>25</v>
@@ -21030,12 +21343,15 @@
         <v>31</v>
       </c>
       <c r="E63" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
+        <v>157</v>
+      </c>
+      <c r="F63" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>230</v>
+        <v>158</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>25</v>
@@ -21047,12 +21363,15 @@
         <v>135</v>
       </c>
       <c r="E64" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+      <c r="F64" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>230</v>
+        <v>158</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>25</v>
@@ -21061,15 +21380,18 @@
         <v>26</v>
       </c>
       <c r="D65" t="s">
-        <v>236</v>
+        <v>31</v>
       </c>
       <c r="E65" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+        <v>260</v>
+      </c>
+      <c r="F65" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>230</v>
+        <v>8</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>25</v>
@@ -21078,15 +21400,18 @@
         <v>26</v>
       </c>
       <c r="D66" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
       <c r="E66" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+        <v>159</v>
+      </c>
+      <c r="F66" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>230</v>
+        <v>8</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>25</v>
@@ -21098,12 +21423,15 @@
         <v>31</v>
       </c>
       <c r="E67" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+        <v>159</v>
+      </c>
+      <c r="F67" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>196</v>
+        <v>8</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>25</v>
@@ -21115,12 +21443,15 @@
         <v>135</v>
       </c>
       <c r="E68" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+        <v>261</v>
+      </c>
+      <c r="F68" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>196</v>
+        <v>8</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>25</v>
@@ -21132,12 +21463,15 @@
         <v>31</v>
       </c>
       <c r="E69" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+        <v>261</v>
+      </c>
+      <c r="F69" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>197</v>
+        <v>7</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>25</v>
@@ -21149,12 +21483,15 @@
         <v>135</v>
       </c>
       <c r="E70" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+        <v>160</v>
+      </c>
+      <c r="F70" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>197</v>
+        <v>7</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>25</v>
@@ -21166,12 +21503,15 @@
         <v>31</v>
       </c>
       <c r="E71" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+        <v>160</v>
+      </c>
+      <c r="F71" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>198</v>
+        <v>7</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>25</v>
@@ -21183,12 +21523,15 @@
         <v>135</v>
       </c>
       <c r="E72" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+        <v>262</v>
+      </c>
+      <c r="F72" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>198</v>
+        <v>7</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>25</v>
@@ -21200,12 +21543,15 @@
         <v>31</v>
       </c>
       <c r="E73" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+        <v>262</v>
+      </c>
+      <c r="F73" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>198</v>
+        <v>22</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>25</v>
@@ -21217,12 +21563,15 @@
         <v>135</v>
       </c>
       <c r="E74" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+        <v>161</v>
+      </c>
+      <c r="F74" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>198</v>
+        <v>22</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>25</v>
@@ -21234,12 +21583,15 @@
         <v>31</v>
       </c>
       <c r="E75" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+        <v>161</v>
+      </c>
+      <c r="F75" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
-        <v>202</v>
+        <v>22</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>25</v>
@@ -21251,12 +21603,15 @@
         <v>135</v>
       </c>
       <c r="E76" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+        <v>263</v>
+      </c>
+      <c r="F76" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>202</v>
+        <v>22</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>25</v>
@@ -21268,12 +21623,15 @@
         <v>31</v>
       </c>
       <c r="E77" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+        <v>263</v>
+      </c>
+      <c r="F77" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>205</v>
+        <v>24</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>25</v>
@@ -21285,12 +21643,15 @@
         <v>135</v>
       </c>
       <c r="E78" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
+        <v>162</v>
+      </c>
+      <c r="F78" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>205</v>
+        <v>24</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>25</v>
@@ -21302,12 +21663,15 @@
         <v>31</v>
       </c>
       <c r="E79" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+        <v>162</v>
+      </c>
+      <c r="F79" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>204</v>
+        <v>24</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>25</v>
@@ -21319,12 +21683,15 @@
         <v>135</v>
       </c>
       <c r="E80" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
+        <v>264</v>
+      </c>
+      <c r="F80" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>204</v>
+        <v>24</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>25</v>
@@ -21336,12 +21703,15 @@
         <v>31</v>
       </c>
       <c r="E81" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
+        <v>264</v>
+      </c>
+      <c r="F81" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>206</v>
+        <v>164</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>25</v>
@@ -21353,12 +21723,15 @@
         <v>135</v>
       </c>
       <c r="E82" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.15">
+        <v>163</v>
+      </c>
+      <c r="F82" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>206</v>
+        <v>164</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>25</v>
@@ -21370,12 +21743,15 @@
         <v>31</v>
       </c>
       <c r="E83" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
+        <v>163</v>
+      </c>
+      <c r="F83" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>203</v>
+        <v>166</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>25</v>
@@ -21387,12 +21763,15 @@
         <v>135</v>
       </c>
       <c r="E84" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
+        <v>165</v>
+      </c>
+      <c r="F84" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>203</v>
+        <v>166</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>25</v>
@@ -21404,12 +21783,15 @@
         <v>31</v>
       </c>
       <c r="E85" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
+        <v>165</v>
+      </c>
+      <c r="F85" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>227</v>
+        <v>166</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>25</v>
@@ -21421,12 +21803,15 @@
         <v>135</v>
       </c>
       <c r="E86" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.15">
+        <v>265</v>
+      </c>
+      <c r="F86" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>227</v>
+        <v>166</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>25</v>
@@ -21438,12 +21823,15 @@
         <v>31</v>
       </c>
       <c r="E87" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.15">
+        <v>265</v>
+      </c>
+      <c r="F87" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
-        <v>227</v>
+        <v>168</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>25</v>
@@ -21455,12 +21843,15 @@
         <v>135</v>
       </c>
       <c r="E88" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.15">
+        <v>167</v>
+      </c>
+      <c r="F88" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>227</v>
+        <v>168</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>25</v>
@@ -21472,12 +21863,15 @@
         <v>31</v>
       </c>
       <c r="E89" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
+        <v>167</v>
+      </c>
+      <c r="F89" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>207</v>
+        <v>168</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>25</v>
@@ -21489,12 +21883,15 @@
         <v>135</v>
       </c>
       <c r="E90" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
+        <v>266</v>
+      </c>
+      <c r="F90" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
-        <v>207</v>
+        <v>168</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>25</v>
@@ -21506,12 +21903,15 @@
         <v>31</v>
       </c>
       <c r="E91" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.15">
+        <v>266</v>
+      </c>
+      <c r="F91" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
-        <v>207</v>
+        <v>170</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>25</v>
@@ -21523,12 +21923,15 @@
         <v>135</v>
       </c>
       <c r="E92" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.15">
+        <v>169</v>
+      </c>
+      <c r="F92" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
-        <v>207</v>
+        <v>170</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>25</v>
@@ -21540,12 +21943,15 @@
         <v>31</v>
       </c>
       <c r="E93" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.15">
+        <v>169</v>
+      </c>
+      <c r="F93" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
-        <v>201</v>
+        <v>170</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>25</v>
@@ -21557,12 +21963,15 @@
         <v>135</v>
       </c>
       <c r="E94" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.15">
+        <v>267</v>
+      </c>
+      <c r="F94" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
-        <v>201</v>
+        <v>170</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>25</v>
@@ -21574,12 +21983,15 @@
         <v>31</v>
       </c>
       <c r="E95" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.15">
+        <v>267</v>
+      </c>
+      <c r="F95" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>25</v>
@@ -21591,12 +22003,15 @@
         <v>135</v>
       </c>
       <c r="E96" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.15">
+        <v>208</v>
+      </c>
+      <c r="F96" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>25</v>
@@ -21608,12 +22023,15 @@
         <v>31</v>
       </c>
       <c r="E97" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.15">
+        <v>229</v>
+      </c>
+      <c r="F97" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>25</v>
@@ -21625,12 +22043,15 @@
         <v>135</v>
       </c>
       <c r="E98" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.15">
+        <v>268</v>
+      </c>
+      <c r="F98" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>25</v>
@@ -21642,12 +22063,15 @@
         <v>31</v>
       </c>
       <c r="E99" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.15">
+        <v>268</v>
+      </c>
+      <c r="F99" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
-        <v>200</v>
+        <v>226</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>25</v>
@@ -21659,243 +22083,1377 @@
         <v>135</v>
       </c>
       <c r="E100" t="s">
+        <v>230</v>
+      </c>
+      <c r="F100" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A101" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C101" t="s">
+        <v>26</v>
+      </c>
+      <c r="D101" t="s">
+        <v>135</v>
+      </c>
+      <c r="E101" t="s">
+        <v>235</v>
+      </c>
+      <c r="F101" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A102" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C102" t="s">
+        <v>26</v>
+      </c>
+      <c r="D102" t="s">
+        <v>31</v>
+      </c>
+      <c r="E102" t="s">
+        <v>230</v>
+      </c>
+      <c r="F102" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A103" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C103" t="s">
+        <v>26</v>
+      </c>
+      <c r="D103" t="s">
+        <v>31</v>
+      </c>
+      <c r="E103" t="s">
+        <v>235</v>
+      </c>
+      <c r="F103" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A104" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C104" t="s">
+        <v>26</v>
+      </c>
+      <c r="D104" t="s">
+        <v>135</v>
+      </c>
+      <c r="E104" t="s">
+        <v>231</v>
+      </c>
+      <c r="F104" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A105" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C105" t="s">
+        <v>26</v>
+      </c>
+      <c r="D105" t="s">
+        <v>31</v>
+      </c>
+      <c r="E105" t="s">
+        <v>231</v>
+      </c>
+      <c r="F105" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A106" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C106" t="s">
+        <v>26</v>
+      </c>
+      <c r="D106" t="s">
+        <v>135</v>
+      </c>
+      <c r="E106" t="s">
+        <v>232</v>
+      </c>
+      <c r="F106" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A107" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C107" t="s">
+        <v>26</v>
+      </c>
+      <c r="D107" t="s">
+        <v>234</v>
+      </c>
+      <c r="E107" t="s">
+        <v>233</v>
+      </c>
+      <c r="F107" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A108" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C108" t="s">
+        <v>26</v>
+      </c>
+      <c r="D108" t="s">
+        <v>31</v>
+      </c>
+      <c r="E108" t="s">
+        <v>232</v>
+      </c>
+      <c r="F108" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A109" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C109" t="s">
+        <v>26</v>
+      </c>
+      <c r="D109" t="s">
+        <v>31</v>
+      </c>
+      <c r="E109" t="s">
+        <v>233</v>
+      </c>
+      <c r="F109" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A110" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C110" t="s">
+        <v>26</v>
+      </c>
+      <c r="D110" t="s">
+        <v>135</v>
+      </c>
+      <c r="E110" t="s">
+        <v>225</v>
+      </c>
+      <c r="F110" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A111" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C111" t="s">
+        <v>26</v>
+      </c>
+      <c r="D111" t="s">
+        <v>31</v>
+      </c>
+      <c r="E111" t="s">
+        <v>225</v>
+      </c>
+      <c r="F111" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A112" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C112" t="s">
+        <v>26</v>
+      </c>
+      <c r="D112" t="s">
+        <v>135</v>
+      </c>
+      <c r="E112" t="s">
+        <v>269</v>
+      </c>
+      <c r="F112" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A113" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C113" t="s">
+        <v>26</v>
+      </c>
+      <c r="D113" t="s">
+        <v>31</v>
+      </c>
+      <c r="E113" t="s">
+        <v>269</v>
+      </c>
+      <c r="F113" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A114" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C114" t="s">
+        <v>26</v>
+      </c>
+      <c r="D114" t="s">
+        <v>135</v>
+      </c>
+      <c r="E114" t="s">
+        <v>209</v>
+      </c>
+      <c r="F114" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A115" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C115" t="s">
+        <v>26</v>
+      </c>
+      <c r="D115" t="s">
+        <v>31</v>
+      </c>
+      <c r="E115" t="s">
+        <v>209</v>
+      </c>
+      <c r="F115" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A116" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C116" t="s">
+        <v>26</v>
+      </c>
+      <c r="D116" t="s">
+        <v>135</v>
+      </c>
+      <c r="E116" t="s">
+        <v>210</v>
+      </c>
+      <c r="F116" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A117" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C117" t="s">
+        <v>26</v>
+      </c>
+      <c r="D117" t="s">
+        <v>31</v>
+      </c>
+      <c r="E117" t="s">
+        <v>210</v>
+      </c>
+      <c r="F117" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A118" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C118" t="s">
+        <v>26</v>
+      </c>
+      <c r="D118" t="s">
+        <v>135</v>
+      </c>
+      <c r="E118" t="s">
+        <v>211</v>
+      </c>
+      <c r="F118" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A119" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C119" t="s">
+        <v>26</v>
+      </c>
+      <c r="D119" t="s">
+        <v>31</v>
+      </c>
+      <c r="E119" t="s">
+        <v>211</v>
+      </c>
+      <c r="F119" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A120" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C120" t="s">
+        <v>26</v>
+      </c>
+      <c r="D120" t="s">
+        <v>135</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F120" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A121" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C121" t="s">
+        <v>26</v>
+      </c>
+      <c r="D121" t="s">
+        <v>31</v>
+      </c>
+      <c r="E121" t="s">
+        <v>270</v>
+      </c>
+      <c r="F121" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A122" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C122" t="s">
+        <v>26</v>
+      </c>
+      <c r="D122" t="s">
+        <v>135</v>
+      </c>
+      <c r="E122" t="s">
+        <v>216</v>
+      </c>
+      <c r="F122" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A123" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C123" t="s">
+        <v>26</v>
+      </c>
+      <c r="D123" t="s">
+        <v>31</v>
+      </c>
+      <c r="E123" t="s">
+        <v>216</v>
+      </c>
+      <c r="F123" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A124" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C124" t="s">
+        <v>26</v>
+      </c>
+      <c r="D124" t="s">
+        <v>135</v>
+      </c>
+      <c r="E124" t="s">
+        <v>271</v>
+      </c>
+      <c r="F124" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A125" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C125" t="s">
+        <v>26</v>
+      </c>
+      <c r="D125" t="s">
+        <v>31</v>
+      </c>
+      <c r="E125" t="s">
+        <v>271</v>
+      </c>
+      <c r="F125" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A126" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C126" t="s">
+        <v>26</v>
+      </c>
+      <c r="D126" t="s">
+        <v>135</v>
+      </c>
+      <c r="E126" t="s">
+        <v>221</v>
+      </c>
+      <c r="F126" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A127" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C127" t="s">
+        <v>26</v>
+      </c>
+      <c r="D127" t="s">
+        <v>31</v>
+      </c>
+      <c r="E127" t="s">
+        <v>221</v>
+      </c>
+      <c r="F127" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A128" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C128" t="s">
+        <v>26</v>
+      </c>
+      <c r="D128" t="s">
+        <v>135</v>
+      </c>
+      <c r="E128" t="s">
+        <v>272</v>
+      </c>
+      <c r="F128" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A129" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C129" t="s">
+        <v>26</v>
+      </c>
+      <c r="D129" t="s">
+        <v>31</v>
+      </c>
+      <c r="E129" t="s">
+        <v>272</v>
+      </c>
+      <c r="F129" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A130" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C130" t="s">
+        <v>26</v>
+      </c>
+      <c r="D130" t="s">
+        <v>135</v>
+      </c>
+      <c r="E130" t="s">
+        <v>220</v>
+      </c>
+      <c r="F130" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A131" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C131" t="s">
+        <v>26</v>
+      </c>
+      <c r="D131" t="s">
+        <v>31</v>
+      </c>
+      <c r="E131" t="s">
+        <v>220</v>
+      </c>
+      <c r="F131" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A132" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C132" t="s">
+        <v>26</v>
+      </c>
+      <c r="D132" t="s">
+        <v>135</v>
+      </c>
+      <c r="E132" t="s">
+        <v>273</v>
+      </c>
+      <c r="F132" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A133" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C133" t="s">
+        <v>26</v>
+      </c>
+      <c r="D133" t="s">
+        <v>31</v>
+      </c>
+      <c r="E133" t="s">
+        <v>273</v>
+      </c>
+      <c r="F133" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A134" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C134" t="s">
+        <v>26</v>
+      </c>
+      <c r="D134" t="s">
+        <v>135</v>
+      </c>
+      <c r="E134" t="s">
+        <v>222</v>
+      </c>
+      <c r="F134" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A135" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C135" t="s">
+        <v>26</v>
+      </c>
+      <c r="D135" t="s">
+        <v>31</v>
+      </c>
+      <c r="E135" t="s">
+        <v>222</v>
+      </c>
+      <c r="F135" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A136" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C136" t="s">
+        <v>26</v>
+      </c>
+      <c r="D136" t="s">
+        <v>135</v>
+      </c>
+      <c r="E136" t="s">
+        <v>274</v>
+      </c>
+      <c r="F136" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A137" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C137" t="s">
+        <v>26</v>
+      </c>
+      <c r="D137" t="s">
+        <v>31</v>
+      </c>
+      <c r="E137" t="s">
+        <v>274</v>
+      </c>
+      <c r="F137" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A138" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C138" t="s">
+        <v>26</v>
+      </c>
+      <c r="D138" t="s">
+        <v>135</v>
+      </c>
+      <c r="E138" t="s">
+        <v>219</v>
+      </c>
+      <c r="F138" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A139" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C139" t="s">
+        <v>26</v>
+      </c>
+      <c r="D139" t="s">
+        <v>31</v>
+      </c>
+      <c r="E139" t="s">
+        <v>219</v>
+      </c>
+      <c r="F139" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A140" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C140" t="s">
+        <v>26</v>
+      </c>
+      <c r="D140" t="s">
+        <v>135</v>
+      </c>
+      <c r="E140" t="s">
+        <v>275</v>
+      </c>
+      <c r="F140" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A141" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C141" t="s">
+        <v>26</v>
+      </c>
+      <c r="D141" t="s">
+        <v>31</v>
+      </c>
+      <c r="E141" t="s">
+        <v>275</v>
+      </c>
+      <c r="F141" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A142" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C142" t="s">
+        <v>26</v>
+      </c>
+      <c r="D142" t="s">
+        <v>135</v>
+      </c>
+      <c r="E142" t="s">
+        <v>217</v>
+      </c>
+      <c r="F142" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A143" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C143" t="s">
+        <v>26</v>
+      </c>
+      <c r="D143" t="s">
+        <v>31</v>
+      </c>
+      <c r="E143" t="s">
+        <v>217</v>
+      </c>
+      <c r="F143" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A144" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C144" t="s">
+        <v>26</v>
+      </c>
+      <c r="D144" t="s">
+        <v>135</v>
+      </c>
+      <c r="E144" t="s">
+        <v>218</v>
+      </c>
+      <c r="F144" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A145" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C145" t="s">
+        <v>26</v>
+      </c>
+      <c r="D145" t="s">
+        <v>31</v>
+      </c>
+      <c r="E145" t="s">
+        <v>218</v>
+      </c>
+      <c r="F145" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A146" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C146" t="s">
+        <v>26</v>
+      </c>
+      <c r="D146" t="s">
+        <v>135</v>
+      </c>
+      <c r="E146" t="s">
+        <v>276</v>
+      </c>
+      <c r="F146" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A147" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C147" t="s">
+        <v>26</v>
+      </c>
+      <c r="D147" t="s">
+        <v>31</v>
+      </c>
+      <c r="E147" t="s">
+        <v>276</v>
+      </c>
+      <c r="F147" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A148" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C148" t="s">
+        <v>26</v>
+      </c>
+      <c r="D148" t="s">
+        <v>135</v>
+      </c>
+      <c r="E148" t="s">
+        <v>223</v>
+      </c>
+      <c r="F148" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A149" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C149" t="s">
+        <v>26</v>
+      </c>
+      <c r="D149" t="s">
+        <v>31</v>
+      </c>
+      <c r="E149" t="s">
+        <v>223</v>
+      </c>
+      <c r="F149" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A150" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C150" t="s">
+        <v>26</v>
+      </c>
+      <c r="D150" t="s">
+        <v>135</v>
+      </c>
+      <c r="E150" t="s">
+        <v>250</v>
+      </c>
+      <c r="F150" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A151" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C151" t="s">
+        <v>26</v>
+      </c>
+      <c r="D151" t="s">
+        <v>31</v>
+      </c>
+      <c r="E151" t="s">
+        <v>224</v>
+      </c>
+      <c r="F151" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A152" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C152" t="s">
+        <v>26</v>
+      </c>
+      <c r="D152" t="s">
+        <v>135</v>
+      </c>
+      <c r="E152" t="s">
+        <v>277</v>
+      </c>
+      <c r="F152" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A153" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C153" t="s">
+        <v>26</v>
+      </c>
+      <c r="D153" t="s">
+        <v>31</v>
+      </c>
+      <c r="E153" t="s">
+        <v>277</v>
+      </c>
+      <c r="F153" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A154" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C154" t="s">
+        <v>26</v>
+      </c>
+      <c r="D154" t="s">
+        <v>135</v>
+      </c>
+      <c r="E154" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A101" s="1" t="s">
+      <c r="F154" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A155" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C155" t="s">
+        <v>26</v>
+      </c>
+      <c r="D155" t="s">
+        <v>31</v>
+      </c>
+      <c r="E155" t="s">
+        <v>215</v>
+      </c>
+      <c r="F155" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A156" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C156" t="s">
+        <v>26</v>
+      </c>
+      <c r="D156" t="s">
+        <v>135</v>
+      </c>
+      <c r="E156" t="s">
+        <v>278</v>
+      </c>
+      <c r="F156" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A157" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C157" t="s">
+        <v>26</v>
+      </c>
+      <c r="D157" t="s">
+        <v>31</v>
+      </c>
+      <c r="E157" t="s">
+        <v>278</v>
+      </c>
+      <c r="F157" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A158" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C158" t="s">
+        <v>26</v>
+      </c>
+      <c r="D158" t="s">
+        <v>135</v>
+      </c>
+      <c r="E158" t="s">
+        <v>212</v>
+      </c>
+      <c r="F158" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A159" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C159" t="s">
+        <v>26</v>
+      </c>
+      <c r="D159" t="s">
+        <v>31</v>
+      </c>
+      <c r="E159" t="s">
+        <v>212</v>
+      </c>
+      <c r="F159" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A160" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C160" t="s">
+        <v>26</v>
+      </c>
+      <c r="D160" t="s">
+        <v>135</v>
+      </c>
+      <c r="E160" t="s">
+        <v>279</v>
+      </c>
+      <c r="F160" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A161" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C161" t="s">
+        <v>26</v>
+      </c>
+      <c r="D161" t="s">
+        <v>31</v>
+      </c>
+      <c r="E161" t="s">
+        <v>279</v>
+      </c>
+      <c r="F161" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A162" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C101" t="s">
-        <v>26</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="B162" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C162" t="s">
+        <v>26</v>
+      </c>
+      <c r="D162" t="s">
+        <v>135</v>
+      </c>
+      <c r="E162" t="s">
+        <v>213</v>
+      </c>
+      <c r="F162" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A163" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C163" t="s">
+        <v>26</v>
+      </c>
+      <c r="D163" t="s">
         <v>31</v>
       </c>
-      <c r="E101" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B104" s="1"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B105" s="1"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B106" s="1"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B107" s="1"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B108" s="1"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B109" s="1"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B110" s="1"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B111" s="1"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B112" s="1"/>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B113" s="1"/>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B114" s="1"/>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B115" s="1"/>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B116" s="1"/>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B117" s="1"/>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B118" s="1"/>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B119" s="1"/>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B120" s="1"/>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B121" s="1"/>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B122" s="1"/>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B123" s="1"/>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B124" s="1"/>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B125" s="1"/>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B126" s="1"/>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B127" s="1"/>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B128" s="1"/>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B129" s="1"/>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B130" s="1"/>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B131" s="1"/>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B132" s="1"/>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B133" s="1"/>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B134" s="1"/>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B135" s="1"/>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B136" s="1"/>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B137" s="1"/>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B138" s="1"/>
-    </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B139" s="1"/>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B140" s="1"/>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B141" s="1"/>
-    </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B142" s="1"/>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B143" s="1"/>
-    </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B144" s="1"/>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B145" s="1"/>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B146" s="1"/>
-    </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B147" s="1"/>
-    </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B148" s="1"/>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B149" s="1"/>
-    </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B150" s="1"/>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B151" s="1"/>
-    </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B152" s="1"/>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B153" s="1"/>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B154" s="1"/>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B155" s="1"/>
-    </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B156" s="1"/>
-    </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B157" s="1"/>
-    </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B158" s="1"/>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B159" s="1"/>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B160" s="1"/>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B161" s="1"/>
-    </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B162" s="1"/>
-    </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B163" s="1"/>
-    </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B164" s="1"/>
-    </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B165" s="1"/>
-    </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B166" s="1"/>
-    </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B167" s="1"/>
-    </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="E163" t="s">
+        <v>213</v>
+      </c>
+      <c r="F163" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A164" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C164" t="s">
+        <v>26</v>
+      </c>
+      <c r="D164" t="s">
+        <v>135</v>
+      </c>
+      <c r="E164" t="s">
+        <v>214</v>
+      </c>
+      <c r="F164" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A165" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C165" t="s">
+        <v>26</v>
+      </c>
+      <c r="D165" t="s">
+        <v>31</v>
+      </c>
+      <c r="E165" t="s">
+        <v>214</v>
+      </c>
+      <c r="F165" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A166" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C166" t="s">
+        <v>26</v>
+      </c>
+      <c r="D166" t="s">
+        <v>135</v>
+      </c>
+      <c r="E166" t="s">
+        <v>280</v>
+      </c>
+      <c r="F166" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A167" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C167" t="s">
+        <v>26</v>
+      </c>
+      <c r="D167" t="s">
+        <v>31</v>
+      </c>
+      <c r="E167" t="s">
+        <v>280</v>
+      </c>
+      <c r="F167" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B168" s="1"/>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B169" s="1"/>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B170" s="1"/>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B171" s="1"/>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B172" s="1"/>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B173" s="1"/>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B174" s="1"/>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B175" s="1"/>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B176" s="1"/>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.15">
@@ -22993,8 +24551,200 @@
     <row r="541" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B541" s="1"/>
     </row>
+    <row r="542" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B542" s="1"/>
+    </row>
+    <row r="543" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B543" s="1"/>
+    </row>
+    <row r="544" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B544" s="1"/>
+    </row>
+    <row r="545" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B545" s="1"/>
+    </row>
+    <row r="546" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B546" s="1"/>
+    </row>
+    <row r="547" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B547" s="1"/>
+    </row>
+    <row r="548" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B548" s="1"/>
+    </row>
+    <row r="549" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B549" s="1"/>
+    </row>
+    <row r="550" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B550" s="1"/>
+    </row>
+    <row r="551" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B551" s="1"/>
+    </row>
+    <row r="552" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B552" s="1"/>
+    </row>
+    <row r="553" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B553" s="1"/>
+    </row>
+    <row r="554" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B554" s="1"/>
+    </row>
+    <row r="555" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B555" s="1"/>
+    </row>
+    <row r="556" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B556" s="1"/>
+    </row>
+    <row r="557" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B557" s="1"/>
+    </row>
+    <row r="558" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B558" s="1"/>
+    </row>
+    <row r="559" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B559" s="1"/>
+    </row>
+    <row r="560" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B560" s="1"/>
+    </row>
+    <row r="561" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B561" s="1"/>
+    </row>
+    <row r="562" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B562" s="1"/>
+    </row>
+    <row r="563" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B563" s="1"/>
+    </row>
+    <row r="564" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B564" s="1"/>
+    </row>
+    <row r="565" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B565" s="1"/>
+    </row>
+    <row r="566" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B566" s="1"/>
+    </row>
+    <row r="567" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B567" s="1"/>
+    </row>
+    <row r="568" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B568" s="1"/>
+    </row>
+    <row r="569" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B569" s="1"/>
+    </row>
+    <row r="570" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B570" s="1"/>
+    </row>
+    <row r="571" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B571" s="1"/>
+    </row>
+    <row r="572" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B572" s="1"/>
+    </row>
+    <row r="573" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B573" s="1"/>
+    </row>
+    <row r="574" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B574" s="1"/>
+    </row>
+    <row r="575" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B575" s="1"/>
+    </row>
+    <row r="576" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B576" s="1"/>
+    </row>
+    <row r="577" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B577" s="1"/>
+    </row>
+    <row r="578" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B578" s="1"/>
+    </row>
+    <row r="579" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B579" s="1"/>
+    </row>
+    <row r="580" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B580" s="1"/>
+    </row>
+    <row r="581" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B581" s="1"/>
+    </row>
+    <row r="582" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B582" s="1"/>
+    </row>
+    <row r="583" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B583" s="1"/>
+    </row>
+    <row r="584" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B584" s="1"/>
+    </row>
+    <row r="585" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B585" s="1"/>
+    </row>
+    <row r="586" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B586" s="1"/>
+    </row>
+    <row r="587" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B587" s="1"/>
+    </row>
+    <row r="588" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B588" s="1"/>
+    </row>
+    <row r="589" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B589" s="1"/>
+    </row>
+    <row r="590" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B590" s="1"/>
+    </row>
+    <row r="591" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B591" s="1"/>
+    </row>
+    <row r="592" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B592" s="1"/>
+    </row>
+    <row r="593" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B593" s="1"/>
+    </row>
+    <row r="594" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B594" s="1"/>
+    </row>
+    <row r="595" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B595" s="1"/>
+    </row>
+    <row r="596" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B596" s="1"/>
+    </row>
+    <row r="597" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B597" s="1"/>
+    </row>
+    <row r="598" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B598" s="1"/>
+    </row>
+    <row r="599" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B599" s="1"/>
+    </row>
+    <row r="600" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B600" s="1"/>
+    </row>
+    <row r="601" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B601" s="1"/>
+    </row>
+    <row r="602" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B602" s="1"/>
+    </row>
+    <row r="603" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B603" s="1"/>
+    </row>
+    <row r="604" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B604" s="1"/>
+    </row>
+    <row r="605" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B605" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E55"/>
+  <autoFilter ref="A1:F167"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23027,7 +24777,7 @@
         <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
@@ -23043,7 +24793,7 @@
         <v>177</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
@@ -23051,7 +24801,7 @@
         <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
@@ -23059,7 +24809,7 @@
         <v>179</v>
       </c>
       <c r="B6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update on 20250327 part 2
</commit_message>
<xml_diff>
--- a/各地组播源汇总/上海.xlsx
+++ b/各地组播源汇总/上海.xlsx
@@ -26312,10 +26312,10 @@
         <v>26</v>
       </c>
       <c r="D287" t="s">
-        <v>135</v>
+        <v>31</v>
       </c>
       <c r="E287" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F287" t="s">
         <v>244</v>
@@ -26332,10 +26332,10 @@
         <v>26</v>
       </c>
       <c r="D288" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
       <c r="E288" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F288" t="s">
         <v>244</v>

</xml_diff>